<commit_message>
Add ERD, ConceptualModel, Fix UCD
</commit_message>
<xml_diff>
--- a/PlanProjekta.xlsx
+++ b/PlanProjekta.xlsx
@@ -24,9 +24,6 @@
     <t>Ime Zadatka</t>
   </si>
   <si>
-    <t>Trajanje</t>
-  </si>
-  <si>
     <t>Početak</t>
   </si>
   <si>
@@ -39,12 +36,6 @@
     <t>Pokretanje projekta</t>
   </si>
   <si>
-    <t>Procjena resursa</t>
-  </si>
-  <si>
-    <t>Plan intervjurianja</t>
-  </si>
-  <si>
     <t>Studija izvedivosti</t>
   </si>
   <si>
@@ -97,6 +88,15 @@
   </si>
   <si>
     <t>Trajanje(dana)</t>
+  </si>
+  <si>
+    <t>Procjena resursa, ciljeva</t>
+  </si>
+  <si>
+    <t>Istraživanje tržišta</t>
+  </si>
+  <si>
+    <t>Trajanje(dani)</t>
   </si>
 </sst>
 </file>
@@ -690,7 +690,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -701,13 +701,13 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.109375" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
     <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="5" width="15.88671875" customWidth="1"/>
@@ -723,33 +723,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>4</v>
-      </c>
       <c r="G1" s="21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="26" t="s">
         <v>2</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="16">
         <v>4</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B3" s="6">
         <v>3</v>
@@ -785,12 +785,12 @@
         <v>45039</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -802,12 +802,12 @@
         <v>45040</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3">
         <v>6</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="10">
         <v>3</v>
@@ -834,12 +834,12 @@
         <v>45043</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" s="8">
         <v>3</v>
@@ -851,12 +851,12 @@
         <v>45046</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3">
         <v>12</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" s="8">
         <v>3</v>
@@ -883,12 +883,12 @@
         <v>45049</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10" s="8">
         <v>3</v>
@@ -900,12 +900,12 @@
         <v>45052</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B11" s="8">
         <v>2</v>
@@ -917,12 +917,12 @@
         <v>45054</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B12" s="8">
         <v>2</v>
@@ -934,12 +934,12 @@
         <v>45056</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13" s="8">
         <v>2</v>
@@ -951,12 +951,12 @@
         <v>45058</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
         <v>18</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B15" s="8">
         <v>2</v>
@@ -983,12 +983,12 @@
         <v>45060</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B16" s="8">
         <v>4</v>
@@ -1000,12 +1000,12 @@
         <v>45064</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B17" s="8">
         <v>3</v>
@@ -1017,12 +1017,12 @@
         <v>45067</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B18" s="8">
         <v>3</v>
@@ -1034,12 +1034,12 @@
         <v>45070</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B19" s="8">
         <v>6</v>
@@ -1051,7 +1051,7 @@
         <v>45076</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>